<commit_message>
new changes for pbi exec and files
</commit_message>
<xml_diff>
--- a/src/b4d_pbi_executive_dashboard/src/b4d_clickup_mayo_v4.xlsx
+++ b/src/b4d_pbi_executive_dashboard/src/b4d_clickup_mayo_v4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\b4d\projects\b4d_analytics\src\b4d_pbi_executive_dashboard\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05DBA76F-B898-49FF-9439-38E527C36CBC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D4FB21C-6E21-4D18-B012-1F18FF0C55FF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5550" yWindow="7110" windowWidth="18810" windowHeight="7350" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -1689,8 +1689,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X96"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X84" sqref="X84"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="W1" sqref="W1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1698,6 +1698,9 @@
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="44.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="32" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="11.42578125" style="2"/>
   </cols>
   <sheetData>
@@ -2656,7 +2659,7 @@
         <v>62</v>
       </c>
       <c r="R17" s="1">
-        <v>45784</v>
+        <v>45777</v>
       </c>
       <c r="S17" s="1">
         <v>45807</v>

</xml_diff>

<commit_message>
new changes in pbi exec
</commit_message>
<xml_diff>
--- a/src/b4d_pbi_executive_dashboard/src/b4d_clickup_mayo_v4.xlsx
+++ b/src/b4d_pbi_executive_dashboard/src/b4d_clickup_mayo_v4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Documents\b4d\projects\b4d_analytics\src\b4d_pbi_executive_dashboard\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B471CEF6-479D-4031-946C-B35CC1C4584D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BA9198-B6AD-4C7E-B882-BE72AB1BB264}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,14 +16,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$96</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$X$95</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1047" uniqueCount="274">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="273">
   <si>
     <t>fact_date</t>
   </si>
@@ -677,9 +677,6 @@
   </si>
   <si>
     <t>ENTEL</t>
-  </si>
-  <si>
-    <t>868e8d6u2</t>
   </si>
   <si>
     <t>868e8dwkf</t>
@@ -1687,16 +1684,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X96"/>
+  <dimension ref="A1:X95"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B28" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="X44" sqref="X44"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="X96" sqref="X96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.140625" customWidth="1"/>
+    <col min="3" max="3" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="15.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.42578125" customWidth="1"/>
     <col min="9" max="9" width="9" customWidth="1"/>
@@ -1705,7 +1702,8 @@
     <col min="18" max="18" width="10" customWidth="1"/>
     <col min="19" max="19" width="12.5703125" customWidth="1"/>
     <col min="20" max="20" width="22.28515625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="11.42578125" style="2"/>
+    <col min="23" max="23" width="10.85546875" customWidth="1"/>
+    <col min="24" max="24" width="9.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
@@ -1779,7 +1777,7 @@
         <v>22</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -1879,7 +1877,7 @@
         <v>30</v>
       </c>
       <c r="M3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N3" t="s">
         <v>42</v>
@@ -2050,7 +2048,7 @@
         <v>30</v>
       </c>
       <c r="M6" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N6" t="s">
         <v>31</v>
@@ -2109,7 +2107,7 @@
         <v>30</v>
       </c>
       <c r="M7" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N7" t="s">
         <v>42</v>
@@ -2233,7 +2231,7 @@
         <v>30</v>
       </c>
       <c r="M9" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N9" t="s">
         <v>42</v>
@@ -2309,7 +2307,7 @@
         <v>179</v>
       </c>
       <c r="C11" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="D11" t="s">
         <v>67</v>
@@ -2333,7 +2331,7 @@
         <v>30</v>
       </c>
       <c r="M11" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O11">
         <v>90113131698</v>
@@ -2648,7 +2646,7 @@
         <v>30</v>
       </c>
       <c r="M17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N17" t="s">
         <v>31</v>
@@ -2866,7 +2864,7 @@
         <v>30</v>
       </c>
       <c r="M21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N21" t="s">
         <v>42</v>
@@ -2895,10 +2893,10 @@
         <v>45808</v>
       </c>
       <c r="B22" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" t="s">
         <v>231</v>
-      </c>
-      <c r="C22" t="s">
-        <v>232</v>
       </c>
       <c r="D22" t="s">
         <v>67</v>
@@ -2945,10 +2943,10 @@
         <v>45808</v>
       </c>
       <c r="B23" t="s">
+        <v>225</v>
+      </c>
+      <c r="C23" t="s">
         <v>226</v>
-      </c>
-      <c r="C23" t="s">
-        <v>227</v>
       </c>
       <c r="D23" t="s">
         <v>67</v>
@@ -2975,7 +2973,7 @@
         <v>30</v>
       </c>
       <c r="M23" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O23">
         <v>90113131698</v>
@@ -2984,7 +2982,7 @@
         <v>32</v>
       </c>
       <c r="Q23" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="T23" s="1">
         <v>45814</v>
@@ -3001,10 +2999,10 @@
         <v>45808</v>
       </c>
       <c r="B24" t="s">
+        <v>228</v>
+      </c>
+      <c r="C24" t="s">
         <v>229</v>
-      </c>
-      <c r="C24" t="s">
-        <v>230</v>
       </c>
       <c r="D24" t="s">
         <v>67</v>
@@ -3075,7 +3073,7 @@
         <v>30</v>
       </c>
       <c r="M25" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N25" t="s">
         <v>42</v>
@@ -3107,7 +3105,7 @@
         <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="D26" t="s">
         <v>67</v>
@@ -3161,7 +3159,7 @@
         <v>45749</v>
       </c>
       <c r="X26" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
@@ -3169,16 +3167,16 @@
         <v>45808</v>
       </c>
       <c r="B27" t="s">
+        <v>238</v>
+      </c>
+      <c r="C27" t="s">
         <v>239</v>
       </c>
-      <c r="C27" t="s">
+      <c r="D27" t="s">
         <v>240</v>
       </c>
-      <c r="D27" t="s">
+      <c r="E27" t="s">
         <v>241</v>
-      </c>
-      <c r="E27" t="s">
-        <v>242</v>
       </c>
       <c r="F27" t="s">
         <v>41</v>
@@ -3281,7 +3279,7 @@
         <v>164</v>
       </c>
       <c r="C29" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="D29" t="s">
         <v>73</v>
@@ -3349,7 +3347,7 @@
         <v>30</v>
       </c>
       <c r="M30" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N30" t="s">
         <v>42</v>
@@ -3414,7 +3412,7 @@
         <v>30</v>
       </c>
       <c r="M31" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N31" t="s">
         <v>42</v>
@@ -3446,16 +3444,16 @@
         <v>45808</v>
       </c>
       <c r="B32" t="s">
+        <v>253</v>
+      </c>
+      <c r="C32" t="s">
         <v>254</v>
       </c>
-      <c r="C32" t="s">
-        <v>255</v>
-      </c>
       <c r="D32" t="s">
+        <v>240</v>
+      </c>
+      <c r="E32" t="s">
         <v>241</v>
-      </c>
-      <c r="E32" t="s">
-        <v>242</v>
       </c>
       <c r="F32" t="s">
         <v>45</v>
@@ -3470,7 +3468,7 @@
         <v>30</v>
       </c>
       <c r="M32" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O32">
         <v>90113131698</v>
@@ -3520,7 +3518,7 @@
         <v>30</v>
       </c>
       <c r="M33" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N33" t="s">
         <v>42</v>
@@ -3576,7 +3574,7 @@
         <v>30</v>
       </c>
       <c r="M34" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N34" t="s">
         <v>42</v>
@@ -3635,7 +3633,7 @@
         <v>30</v>
       </c>
       <c r="M35" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N35" t="s">
         <v>31</v>
@@ -3700,7 +3698,7 @@
         <v>30</v>
       </c>
       <c r="M36" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N36" t="s">
         <v>42</v>
@@ -3815,7 +3813,7 @@
         <v>30</v>
       </c>
       <c r="M38" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N38" t="s">
         <v>42</v>
@@ -3847,13 +3845,13 @@
         <v>45808</v>
       </c>
       <c r="B39" t="s">
+        <v>218</v>
+      </c>
+      <c r="C39" t="s">
         <v>219</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D39" t="s">
         <v>220</v>
-      </c>
-      <c r="D39" t="s">
-        <v>221</v>
       </c>
       <c r="F39" t="s">
         <v>45</v>
@@ -3868,7 +3866,7 @@
         <v>30</v>
       </c>
       <c r="M39" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N39" t="s">
         <v>42</v>
@@ -3903,7 +3901,7 @@
         <v>45808</v>
       </c>
       <c r="B40" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="C40" t="s">
         <v>216</v>
@@ -3915,10 +3913,10 @@
         <v>59</v>
       </c>
       <c r="F40" t="s">
-        <v>27</v>
+        <v>60</v>
       </c>
       <c r="I40">
-        <v>1283400</v>
+        <v>1328400</v>
       </c>
       <c r="J40" t="s">
         <v>28</v>
@@ -3929,6 +3927,9 @@
       <c r="L40" t="s">
         <v>30</v>
       </c>
+      <c r="M40" t="s">
+        <v>265</v>
+      </c>
       <c r="N40" t="s">
         <v>31</v>
       </c>
@@ -3941,8 +3942,8 @@
       <c r="Q40" t="s">
         <v>217</v>
       </c>
-      <c r="R40" s="1">
-        <v>45807</v>
+      <c r="S40" s="1">
+        <v>45869</v>
       </c>
       <c r="T40" s="1">
         <v>45813</v>
@@ -3965,22 +3966,28 @@
         <v>45808</v>
       </c>
       <c r="B41" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="C41" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="D41" t="s">
-        <v>58</v>
+        <v>25</v>
       </c>
       <c r="E41" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="F41" t="s">
-        <v>60</v>
+        <v>81</v>
+      </c>
+      <c r="G41">
+        <v>18000</v>
+      </c>
+      <c r="H41">
+        <v>25000</v>
       </c>
       <c r="I41">
-        <v>1328400</v>
+        <v>5000</v>
       </c>
       <c r="J41" t="s">
         <v>28</v>
@@ -3992,7 +3999,7 @@
         <v>30</v>
       </c>
       <c r="M41" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N41" t="s">
         <v>31</v>
@@ -4004,22 +4011,13 @@
         <v>32</v>
       </c>
       <c r="Q41" t="s">
-        <v>217</v>
-      </c>
-      <c r="S41" s="1">
-        <v>45869</v>
+        <v>144</v>
       </c>
       <c r="T41" s="1">
-        <v>45813</v>
-      </c>
-      <c r="U41" s="1">
-        <v>45838</v>
-      </c>
-      <c r="V41" s="1">
-        <v>45748</v>
+        <v>45807</v>
       </c>
       <c r="W41" s="1">
-        <v>45814</v>
+        <v>45808</v>
       </c>
       <c r="X41" s="2">
         <v>0</v>
@@ -4030,10 +4028,10 @@
         <v>45808</v>
       </c>
       <c r="B42" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="C42" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="D42" t="s">
         <v>25</v>
@@ -4045,13 +4043,13 @@
         <v>81</v>
       </c>
       <c r="G42">
-        <v>18000</v>
+        <v>38261</v>
       </c>
       <c r="H42">
-        <v>25000</v>
+        <v>0</v>
       </c>
       <c r="I42">
-        <v>5000</v>
+        <v>0</v>
       </c>
       <c r="J42" t="s">
         <v>28</v>
@@ -4063,7 +4061,7 @@
         <v>30</v>
       </c>
       <c r="M42" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N42" t="s">
         <v>31</v>
@@ -4092,10 +4090,10 @@
         <v>45808</v>
       </c>
       <c r="B43" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
       <c r="C43" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="D43" t="s">
         <v>25</v>
@@ -4104,16 +4102,16 @@
         <v>26</v>
       </c>
       <c r="F43" t="s">
-        <v>81</v>
+        <v>27</v>
       </c>
       <c r="G43">
-        <v>38261</v>
+        <v>0</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>4135</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>4135</v>
       </c>
       <c r="J43" t="s">
         <v>28</v>
@@ -4125,10 +4123,7 @@
         <v>30</v>
       </c>
       <c r="M43" t="s">
-        <v>266</v>
-      </c>
-      <c r="N43" t="s">
-        <v>31</v>
+        <v>265</v>
       </c>
       <c r="O43">
         <v>90113131698</v>
@@ -4139,8 +4134,14 @@
       <c r="Q43" t="s">
         <v>144</v>
       </c>
+      <c r="R43" s="1">
+        <v>45807</v>
+      </c>
       <c r="T43" s="1">
-        <v>45807</v>
+        <v>45716</v>
+      </c>
+      <c r="U43" s="1">
+        <v>45835</v>
       </c>
       <c r="W43" s="1">
         <v>45808</v>
@@ -4154,10 +4155,10 @@
         <v>45808</v>
       </c>
       <c r="B44" t="s">
-        <v>142</v>
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>143</v>
+        <v>40</v>
       </c>
       <c r="D44" t="s">
         <v>25</v>
@@ -4166,16 +4167,7 @@
         <v>26</v>
       </c>
       <c r="F44" t="s">
-        <v>27</v>
-      </c>
-      <c r="G44">
-        <v>0</v>
-      </c>
-      <c r="H44">
-        <v>4135</v>
-      </c>
-      <c r="I44">
-        <v>4135</v>
+        <v>41</v>
       </c>
       <c r="J44" t="s">
         <v>28</v>
@@ -4187,7 +4179,10 @@
         <v>30</v>
       </c>
       <c r="M44" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="N44" t="s">
+        <v>42</v>
       </c>
       <c r="O44">
         <v>90113131698</v>
@@ -4196,22 +4191,19 @@
         <v>32</v>
       </c>
       <c r="Q44" t="s">
-        <v>144</v>
-      </c>
-      <c r="R44" s="1">
-        <v>45807</v>
+        <v>40</v>
       </c>
       <c r="T44" s="1">
-        <v>45716</v>
+        <v>45664</v>
       </c>
       <c r="U44" s="1">
-        <v>45835</v>
+        <v>45723</v>
       </c>
       <c r="W44" s="1">
-        <v>45808</v>
+        <v>45717</v>
       </c>
       <c r="X44" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45" spans="1:24" x14ac:dyDescent="0.25">
@@ -4219,10 +4211,10 @@
         <v>45808</v>
       </c>
       <c r="B45" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
       <c r="C45" t="s">
-        <v>40</v>
+        <v>269</v>
       </c>
       <c r="D45" t="s">
         <v>25</v>
@@ -4231,7 +4223,13 @@
         <v>26</v>
       </c>
       <c r="F45" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="G45">
+        <v>1000</v>
+      </c>
+      <c r="H45">
+        <v>17890</v>
       </c>
       <c r="J45" t="s">
         <v>28</v>
@@ -4240,10 +4238,10 @@
         <v>29</v>
       </c>
       <c r="L45" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="M45" t="s">
-        <v>266</v>
+        <v>69</v>
       </c>
       <c r="N45" t="s">
         <v>42</v>
@@ -4255,16 +4253,16 @@
         <v>32</v>
       </c>
       <c r="Q45" t="s">
-        <v>40</v>
+        <v>157</v>
+      </c>
+      <c r="S45" s="1">
+        <v>45820</v>
       </c>
       <c r="T45" s="1">
-        <v>45664</v>
-      </c>
-      <c r="U45" s="1">
-        <v>45723</v>
+        <v>45747</v>
       </c>
       <c r="W45" s="1">
-        <v>45717</v>
+        <v>45749</v>
       </c>
       <c r="X45" s="2">
         <v>0</v>
@@ -4275,40 +4273,37 @@
         <v>45808</v>
       </c>
       <c r="B46" t="s">
-        <v>156</v>
+        <v>232</v>
       </c>
       <c r="C46" t="s">
-        <v>270</v>
+        <v>233</v>
       </c>
       <c r="D46" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E46" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F46" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="G46">
-        <v>1000</v>
+        <v>8000</v>
       </c>
       <c r="H46">
-        <v>17890</v>
+        <v>15000</v>
+      </c>
+      <c r="I46">
+        <v>3000</v>
       </c>
       <c r="J46" t="s">
         <v>28</v>
       </c>
-      <c r="K46" t="s">
-        <v>29</v>
-      </c>
       <c r="L46" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="M46" t="s">
-        <v>69</v>
-      </c>
-      <c r="N46" t="s">
-        <v>42</v>
+        <v>265</v>
       </c>
       <c r="O46">
         <v>90113131698</v>
@@ -4316,17 +4311,14 @@
       <c r="P46" t="s">
         <v>32</v>
       </c>
-      <c r="Q46" t="s">
-        <v>157</v>
-      </c>
       <c r="S46" s="1">
-        <v>45820</v>
+        <v>45869</v>
       </c>
       <c r="T46" s="1">
-        <v>45747</v>
+        <v>45814</v>
       </c>
       <c r="W46" s="1">
-        <v>45749</v>
+        <v>45815</v>
       </c>
       <c r="X46" s="2">
         <v>0</v>
@@ -4337,37 +4329,40 @@
         <v>45808</v>
       </c>
       <c r="B47" t="s">
-        <v>233</v>
+        <v>121</v>
       </c>
       <c r="C47" t="s">
-        <v>234</v>
+        <v>122</v>
       </c>
       <c r="D47" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E47" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="F47" t="s">
         <v>81</v>
       </c>
       <c r="G47">
-        <v>8000</v>
+        <v>15480</v>
       </c>
       <c r="H47">
-        <v>15000</v>
-      </c>
-      <c r="I47">
-        <v>3000</v>
+        <v>16416</v>
       </c>
       <c r="J47" t="s">
         <v>28</v>
       </c>
+      <c r="K47" t="s">
+        <v>29</v>
+      </c>
       <c r="L47" t="s">
         <v>30</v>
       </c>
       <c r="M47" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="N47" t="s">
+        <v>42</v>
       </c>
       <c r="O47">
         <v>90113131698</v>
@@ -4375,14 +4370,20 @@
       <c r="P47" t="s">
         <v>32</v>
       </c>
+      <c r="Q47" t="s">
+        <v>122</v>
+      </c>
       <c r="S47" s="1">
-        <v>45869</v>
+        <v>45799</v>
       </c>
       <c r="T47" s="1">
-        <v>45814</v>
+        <v>45715</v>
+      </c>
+      <c r="U47" s="1">
+        <v>45714</v>
       </c>
       <c r="W47" s="1">
-        <v>45815</v>
+        <v>45717</v>
       </c>
       <c r="X47" s="2">
         <v>0</v>
@@ -4393,10 +4394,10 @@
         <v>45808</v>
       </c>
       <c r="B48" t="s">
-        <v>121</v>
+        <v>242</v>
       </c>
       <c r="C48" t="s">
-        <v>122</v>
+        <v>243</v>
       </c>
       <c r="D48" t="s">
         <v>25</v>
@@ -4405,13 +4406,13 @@
         <v>26</v>
       </c>
       <c r="F48" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="G48">
-        <v>15480</v>
+        <v>7000</v>
       </c>
       <c r="H48">
-        <v>16416</v>
+        <v>15000</v>
       </c>
       <c r="J48" t="s">
         <v>28</v>
@@ -4423,7 +4424,7 @@
         <v>30</v>
       </c>
       <c r="M48" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N48" t="s">
         <v>42</v>
@@ -4435,19 +4436,10 @@
         <v>32</v>
       </c>
       <c r="Q48" t="s">
-        <v>122</v>
-      </c>
-      <c r="S48" s="1">
-        <v>45799</v>
+        <v>244</v>
       </c>
       <c r="T48" s="1">
-        <v>45715</v>
-      </c>
-      <c r="U48" s="1">
-        <v>45714</v>
-      </c>
-      <c r="W48" s="1">
-        <v>45717</v>
+        <v>45819</v>
       </c>
       <c r="X48" s="2">
         <v>0</v>
@@ -4458,10 +4450,10 @@
         <v>45808</v>
       </c>
       <c r="B49" t="s">
-        <v>243</v>
+        <v>257</v>
       </c>
       <c r="C49" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="D49" t="s">
         <v>25</v>
@@ -4473,10 +4465,10 @@
         <v>45</v>
       </c>
       <c r="G49">
-        <v>7000</v>
+        <v>4500</v>
       </c>
       <c r="H49">
-        <v>15000</v>
+        <v>700</v>
       </c>
       <c r="J49" t="s">
         <v>28</v>
@@ -4488,7 +4480,7 @@
         <v>30</v>
       </c>
       <c r="M49" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N49" t="s">
         <v>42</v>
@@ -4500,7 +4492,7 @@
         <v>32</v>
       </c>
       <c r="Q49" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="T49" s="1">
         <v>45819</v>
@@ -4514,10 +4506,10 @@
         <v>45808</v>
       </c>
       <c r="B50" t="s">
-        <v>258</v>
+        <v>23</v>
       </c>
       <c r="C50" t="s">
-        <v>259</v>
+        <v>24</v>
       </c>
       <c r="D50" t="s">
         <v>25</v>
@@ -4526,13 +4518,13 @@
         <v>26</v>
       </c>
       <c r="F50" t="s">
-        <v>45</v>
+        <v>27</v>
       </c>
       <c r="G50">
-        <v>4500</v>
+        <v>22781.85</v>
       </c>
       <c r="H50">
-        <v>700</v>
+        <v>37618.769999999997</v>
       </c>
       <c r="J50" t="s">
         <v>28</v>
@@ -4544,10 +4536,10 @@
         <v>30</v>
       </c>
       <c r="M50" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N50" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="O50">
         <v>90113131698</v>
@@ -4556,10 +4548,19 @@
         <v>32</v>
       </c>
       <c r="Q50" t="s">
-        <v>245</v>
+        <v>24</v>
+      </c>
+      <c r="R50" s="1">
+        <v>45740</v>
       </c>
       <c r="T50" s="1">
-        <v>45819</v>
+        <v>45662</v>
+      </c>
+      <c r="U50" s="1">
+        <v>45594</v>
+      </c>
+      <c r="W50" s="1">
+        <v>45717</v>
       </c>
       <c r="X50" s="2">
         <v>0</v>
@@ -4570,25 +4571,19 @@
         <v>45808</v>
       </c>
       <c r="B51" t="s">
-        <v>23</v>
+        <v>192</v>
       </c>
       <c r="C51" t="s">
-        <v>24</v>
+        <v>193</v>
       </c>
       <c r="D51" t="s">
-        <v>25</v>
+        <v>188</v>
       </c>
       <c r="E51" t="s">
         <v>26</v>
       </c>
       <c r="F51" t="s">
-        <v>27</v>
-      </c>
-      <c r="G51">
-        <v>22781.85</v>
-      </c>
-      <c r="H51">
-        <v>37618.769999999997</v>
+        <v>41</v>
       </c>
       <c r="J51" t="s">
         <v>28</v>
@@ -4600,10 +4595,10 @@
         <v>30</v>
       </c>
       <c r="M51" t="s">
-        <v>266</v>
+        <v>69</v>
       </c>
       <c r="N51" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="O51">
         <v>90113131698</v>
@@ -4611,20 +4606,11 @@
       <c r="P51" t="s">
         <v>32</v>
       </c>
-      <c r="Q51" t="s">
-        <v>24</v>
-      </c>
-      <c r="R51" s="1">
-        <v>45740</v>
-      </c>
       <c r="T51" s="1">
-        <v>45662</v>
-      </c>
-      <c r="U51" s="1">
-        <v>45594</v>
+        <v>45768</v>
       </c>
       <c r="W51" s="1">
-        <v>45717</v>
+        <v>45769</v>
       </c>
       <c r="X51" s="2">
         <v>0</v>
@@ -4635,16 +4621,16 @@
         <v>45808</v>
       </c>
       <c r="B52" t="s">
-        <v>192</v>
+        <v>108</v>
       </c>
       <c r="C52" t="s">
-        <v>193</v>
+        <v>109</v>
       </c>
       <c r="D52" t="s">
-        <v>188</v>
+        <v>58</v>
       </c>
       <c r="E52" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F52" t="s">
         <v>41</v>
@@ -4659,7 +4645,7 @@
         <v>30</v>
       </c>
       <c r="M52" t="s">
-        <v>69</v>
+        <v>265</v>
       </c>
       <c r="N52" t="s">
         <v>42</v>
@@ -4670,11 +4656,17 @@
       <c r="P52" t="s">
         <v>32</v>
       </c>
+      <c r="Q52" t="s">
+        <v>36</v>
+      </c>
       <c r="T52" s="1">
-        <v>45768</v>
+        <v>45712</v>
+      </c>
+      <c r="U52" s="1">
+        <v>45712</v>
       </c>
       <c r="W52" s="1">
-        <v>45769</v>
+        <v>45717</v>
       </c>
       <c r="X52" s="2">
         <v>0</v>
@@ -4685,19 +4677,22 @@
         <v>45808</v>
       </c>
       <c r="B53" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
       <c r="C53" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
       <c r="D53" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
       <c r="E53" t="s">
         <v>59</v>
       </c>
       <c r="F53" t="s">
-        <v>41</v>
+        <v>98</v>
+      </c>
+      <c r="G53">
+        <v>5000</v>
       </c>
       <c r="J53" t="s">
         <v>28</v>
@@ -4709,10 +4704,7 @@
         <v>30</v>
       </c>
       <c r="M53" t="s">
-        <v>266</v>
-      </c>
-      <c r="N53" t="s">
-        <v>42</v>
+        <v>265</v>
       </c>
       <c r="O53">
         <v>90113131698</v>
@@ -4720,17 +4712,11 @@
       <c r="P53" t="s">
         <v>32</v>
       </c>
-      <c r="Q53" t="s">
-        <v>36</v>
-      </c>
       <c r="T53" s="1">
-        <v>45712</v>
-      </c>
-      <c r="U53" s="1">
-        <v>45712</v>
+        <v>45701</v>
       </c>
       <c r="W53" s="1">
-        <v>45717</v>
+        <v>45804</v>
       </c>
       <c r="X53" s="2">
         <v>0</v>
@@ -4741,10 +4727,10 @@
         <v>45808</v>
       </c>
       <c r="B54" t="s">
-        <v>96</v>
+        <v>148</v>
       </c>
       <c r="C54" t="s">
-        <v>97</v>
+        <v>149</v>
       </c>
       <c r="D54" t="s">
         <v>67</v>
@@ -4753,10 +4739,13 @@
         <v>59</v>
       </c>
       <c r="F54" t="s">
-        <v>98</v>
+        <v>60</v>
       </c>
       <c r="G54">
-        <v>5000</v>
+        <v>10557</v>
+      </c>
+      <c r="H54">
+        <v>10500</v>
       </c>
       <c r="J54" t="s">
         <v>28</v>
@@ -4764,11 +4753,8 @@
       <c r="K54" t="s">
         <v>29</v>
       </c>
-      <c r="L54" t="s">
-        <v>30</v>
-      </c>
       <c r="M54" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O54">
         <v>90113131698</v>
@@ -4776,11 +4762,20 @@
       <c r="P54" t="s">
         <v>32</v>
       </c>
+      <c r="Q54" t="s">
+        <v>150</v>
+      </c>
+      <c r="S54" s="1">
+        <v>45869</v>
+      </c>
       <c r="T54" s="1">
-        <v>45701</v>
+        <v>45716</v>
+      </c>
+      <c r="U54" s="1">
+        <v>45810</v>
       </c>
       <c r="W54" s="1">
-        <v>45804</v>
+        <v>45749</v>
       </c>
       <c r="X54" s="2">
         <v>0</v>
@@ -4791,34 +4786,19 @@
         <v>45808</v>
       </c>
       <c r="B55" t="s">
-        <v>148</v>
+        <v>203</v>
       </c>
       <c r="C55" t="s">
-        <v>149</v>
+        <v>204</v>
       </c>
       <c r="D55" t="s">
-        <v>67</v>
+        <v>200</v>
       </c>
       <c r="E55" t="s">
         <v>59</v>
       </c>
       <c r="F55" t="s">
-        <v>60</v>
-      </c>
-      <c r="G55">
-        <v>10557</v>
-      </c>
-      <c r="H55">
-        <v>10500</v>
-      </c>
-      <c r="J55" t="s">
-        <v>28</v>
-      </c>
-      <c r="K55" t="s">
-        <v>29</v>
-      </c>
-      <c r="M55" t="s">
-        <v>266</v>
+        <v>41</v>
       </c>
       <c r="O55">
         <v>90113131698</v>
@@ -4826,20 +4806,11 @@
       <c r="P55" t="s">
         <v>32</v>
       </c>
-      <c r="Q55" t="s">
-        <v>150</v>
-      </c>
-      <c r="S55" s="1">
-        <v>45869</v>
-      </c>
       <c r="T55" s="1">
-        <v>45716</v>
-      </c>
-      <c r="U55" s="1">
-        <v>45810</v>
+        <v>45790</v>
       </c>
       <c r="W55" s="1">
-        <v>45749</v>
+        <v>45791</v>
       </c>
       <c r="X55" s="2">
         <v>0</v>
@@ -4850,19 +4821,40 @@
         <v>45808</v>
       </c>
       <c r="B56" t="s">
-        <v>203</v>
+        <v>47</v>
       </c>
       <c r="C56" t="s">
-        <v>204</v>
+        <v>48</v>
       </c>
       <c r="D56" t="s">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="E56" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="F56" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="G56">
+        <v>5000</v>
+      </c>
+      <c r="H56">
+        <v>10000</v>
+      </c>
+      <c r="J56" t="s">
+        <v>28</v>
+      </c>
+      <c r="K56" t="s">
+        <v>29</v>
+      </c>
+      <c r="L56" t="s">
+        <v>30</v>
+      </c>
+      <c r="M56" t="s">
+        <v>265</v>
+      </c>
+      <c r="N56" t="s">
+        <v>31</v>
       </c>
       <c r="O56">
         <v>90113131698</v>
@@ -4871,10 +4863,13 @@
         <v>32</v>
       </c>
       <c r="T56" s="1">
-        <v>45790</v>
+        <v>45664</v>
+      </c>
+      <c r="V56" s="1">
+        <v>45748</v>
       </c>
       <c r="W56" s="1">
-        <v>45791</v>
+        <v>45749</v>
       </c>
       <c r="X56" s="2">
         <v>0</v>
@@ -4885,10 +4880,10 @@
         <v>45808</v>
       </c>
       <c r="B57" t="s">
-        <v>47</v>
+        <v>140</v>
       </c>
       <c r="C57" t="s">
-        <v>48</v>
+        <v>141</v>
       </c>
       <c r="D57" t="s">
         <v>25</v>
@@ -4897,13 +4892,13 @@
         <v>26</v>
       </c>
       <c r="F57" t="s">
-        <v>35</v>
+        <v>45</v>
       </c>
       <c r="G57">
-        <v>5000</v>
+        <v>7000</v>
       </c>
       <c r="H57">
-        <v>10000</v>
+        <v>17000</v>
       </c>
       <c r="J57" t="s">
         <v>28</v>
@@ -4912,13 +4907,13 @@
         <v>29</v>
       </c>
       <c r="L57" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="M57" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N57" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="O57">
         <v>90113131698</v>
@@ -4926,11 +4921,14 @@
       <c r="P57" t="s">
         <v>32</v>
       </c>
+      <c r="Q57" t="s">
+        <v>117</v>
+      </c>
       <c r="T57" s="1">
-        <v>45664</v>
-      </c>
-      <c r="V57" s="1">
-        <v>45748</v>
+        <v>45716</v>
+      </c>
+      <c r="U57" s="1">
+        <v>45699</v>
       </c>
       <c r="W57" s="1">
         <v>45749</v>
@@ -4944,40 +4942,34 @@
         <v>45808</v>
       </c>
       <c r="B58" t="s">
-        <v>140</v>
+        <v>223</v>
       </c>
       <c r="C58" t="s">
-        <v>141</v>
+        <v>224</v>
       </c>
       <c r="D58" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E58" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F58" t="s">
         <v>45</v>
       </c>
       <c r="G58">
-        <v>7000</v>
+        <v>2500</v>
       </c>
       <c r="H58">
-        <v>17000</v>
+        <v>15000</v>
       </c>
       <c r="J58" t="s">
         <v>28</v>
       </c>
-      <c r="K58" t="s">
-        <v>29</v>
-      </c>
       <c r="L58" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="M58" t="s">
-        <v>266</v>
-      </c>
-      <c r="N58" t="s">
-        <v>42</v>
+        <v>69</v>
       </c>
       <c r="O58">
         <v>90113131698</v>
@@ -4986,16 +4978,13 @@
         <v>32</v>
       </c>
       <c r="Q58" t="s">
-        <v>117</v>
+        <v>88</v>
       </c>
       <c r="T58" s="1">
-        <v>45716</v>
-      </c>
-      <c r="U58" s="1">
-        <v>45699</v>
+        <v>45814</v>
       </c>
       <c r="W58" s="1">
-        <v>45749</v>
+        <v>45815</v>
       </c>
       <c r="X58" s="2">
         <v>0</v>
@@ -5006,35 +4995,41 @@
         <v>45808</v>
       </c>
       <c r="B59" t="s">
-        <v>224</v>
+        <v>131</v>
       </c>
       <c r="C59" t="s">
-        <v>225</v>
+        <v>132</v>
       </c>
       <c r="D59" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E59" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="F59" t="s">
-        <v>45</v>
+        <v>81</v>
       </c>
       <c r="G59">
-        <v>2500</v>
+        <v>5382</v>
       </c>
       <c r="H59">
-        <v>15000</v>
+        <v>9286</v>
       </c>
       <c r="J59" t="s">
         <v>28</v>
       </c>
+      <c r="K59" t="s">
+        <v>29</v>
+      </c>
       <c r="L59" t="s">
         <v>30</v>
       </c>
       <c r="M59" t="s">
         <v>69</v>
       </c>
+      <c r="N59" t="s">
+        <v>42</v>
+      </c>
       <c r="O59">
         <v>90113131698</v>
       </c>
@@ -5042,13 +5037,19 @@
         <v>32</v>
       </c>
       <c r="Q59" t="s">
-        <v>88</v>
+        <v>132</v>
+      </c>
+      <c r="S59" s="1">
+        <v>45789</v>
       </c>
       <c r="T59" s="1">
-        <v>45814</v>
+        <v>45715</v>
+      </c>
+      <c r="U59" s="1">
+        <v>45775</v>
       </c>
       <c r="W59" s="1">
-        <v>45815</v>
+        <v>45749</v>
       </c>
       <c r="X59" s="2">
         <v>0</v>
@@ -5059,10 +5060,10 @@
         <v>45808</v>
       </c>
       <c r="B60" t="s">
-        <v>131</v>
+        <v>208</v>
       </c>
       <c r="C60" t="s">
-        <v>132</v>
+        <v>209</v>
       </c>
       <c r="D60" t="s">
         <v>25</v>
@@ -5071,13 +5072,13 @@
         <v>26</v>
       </c>
       <c r="F60" t="s">
-        <v>81</v>
+        <v>45</v>
       </c>
       <c r="G60">
-        <v>5382</v>
+        <v>13000</v>
       </c>
       <c r="H60">
-        <v>9286</v>
+        <v>20000</v>
       </c>
       <c r="J60" t="s">
         <v>28</v>
@@ -5089,7 +5090,7 @@
         <v>30</v>
       </c>
       <c r="M60" t="s">
-        <v>69</v>
+        <v>265</v>
       </c>
       <c r="N60" t="s">
         <v>42</v>
@@ -5101,19 +5102,13 @@
         <v>32</v>
       </c>
       <c r="Q60" t="s">
-        <v>132</v>
-      </c>
-      <c r="S60" s="1">
-        <v>45789</v>
+        <v>209</v>
       </c>
       <c r="T60" s="1">
-        <v>45715</v>
-      </c>
-      <c r="U60" s="1">
-        <v>45775</v>
+        <v>45807</v>
       </c>
       <c r="W60" s="1">
-        <v>45749</v>
+        <v>45808</v>
       </c>
       <c r="X60" s="2">
         <v>0</v>
@@ -5124,25 +5119,19 @@
         <v>45808</v>
       </c>
       <c r="B61" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="C61" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="D61" t="s">
-        <v>25</v>
+        <v>188</v>
       </c>
       <c r="E61" t="s">
         <v>26</v>
       </c>
       <c r="F61" t="s">
-        <v>45</v>
-      </c>
-      <c r="G61">
-        <v>13000</v>
-      </c>
-      <c r="H61">
-        <v>20000</v>
+        <v>41</v>
       </c>
       <c r="J61" t="s">
         <v>28</v>
@@ -5154,7 +5143,7 @@
         <v>30</v>
       </c>
       <c r="M61" t="s">
-        <v>266</v>
+        <v>69</v>
       </c>
       <c r="N61" t="s">
         <v>42</v>
@@ -5165,14 +5154,11 @@
       <c r="P61" t="s">
         <v>32</v>
       </c>
-      <c r="Q61" t="s">
-        <v>209</v>
-      </c>
       <c r="T61" s="1">
-        <v>45807</v>
+        <v>45768</v>
       </c>
       <c r="W61" s="1">
-        <v>45808</v>
+        <v>45769</v>
       </c>
       <c r="X61" s="2">
         <v>0</v>
@@ -5183,10 +5169,10 @@
         <v>45808</v>
       </c>
       <c r="B62" t="s">
-        <v>186</v>
+        <v>194</v>
       </c>
       <c r="C62" t="s">
-        <v>187</v>
+        <v>195</v>
       </c>
       <c r="D62" t="s">
         <v>188</v>
@@ -5233,28 +5219,28 @@
         <v>45808</v>
       </c>
       <c r="B63" t="s">
-        <v>194</v>
+        <v>71</v>
       </c>
       <c r="C63" t="s">
-        <v>195</v>
+        <v>72</v>
       </c>
       <c r="D63" t="s">
-        <v>188</v>
+        <v>73</v>
       </c>
       <c r="E63" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F63" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="J63" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="K63" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="L63" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="M63" t="s">
         <v>69</v>
@@ -5268,11 +5254,20 @@
       <c r="P63" t="s">
         <v>32</v>
       </c>
+      <c r="Q63" t="s">
+        <v>76</v>
+      </c>
+      <c r="R63" s="1">
+        <v>45740</v>
+      </c>
       <c r="T63" s="1">
-        <v>45768</v>
+        <v>45694</v>
+      </c>
+      <c r="U63" s="1">
+        <v>45701</v>
       </c>
       <c r="W63" s="1">
-        <v>45769</v>
+        <v>45717</v>
       </c>
       <c r="X63" s="2">
         <v>0</v>
@@ -5283,34 +5278,28 @@
         <v>45808</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>84</v>
       </c>
       <c r="C64" t="s">
-        <v>72</v>
+        <v>85</v>
       </c>
       <c r="D64" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E64" t="s">
         <v>59</v>
       </c>
       <c r="F64" t="s">
-        <v>27</v>
+        <v>41</v>
       </c>
       <c r="J64" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="K64" t="s">
-        <v>68</v>
-      </c>
-      <c r="L64" t="s">
-        <v>75</v>
+        <v>29</v>
       </c>
       <c r="M64" t="s">
-        <v>69</v>
-      </c>
-      <c r="N64" t="s">
-        <v>42</v>
+        <v>265</v>
       </c>
       <c r="O64">
         <v>90113131698</v>
@@ -5319,15 +5308,9 @@
         <v>32</v>
       </c>
       <c r="Q64" t="s">
-        <v>76</v>
-      </c>
-      <c r="R64" s="1">
-        <v>45740</v>
+        <v>36</v>
       </c>
       <c r="T64" s="1">
-        <v>45694</v>
-      </c>
-      <c r="U64" s="1">
         <v>45701</v>
       </c>
       <c r="W64" s="1">
@@ -5342,13 +5325,13 @@
         <v>45808</v>
       </c>
       <c r="B65" t="s">
-        <v>84</v>
+        <v>181</v>
       </c>
       <c r="C65" t="s">
-        <v>85</v>
+        <v>182</v>
       </c>
       <c r="D65" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E65" t="s">
         <v>59</v>
@@ -5356,14 +5339,11 @@
       <c r="F65" t="s">
         <v>41</v>
       </c>
-      <c r="J65" t="s">
-        <v>28</v>
-      </c>
-      <c r="K65" t="s">
-        <v>29</v>
+      <c r="H65">
+        <v>10000</v>
       </c>
       <c r="M65" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O65">
         <v>90113131698</v>
@@ -5371,14 +5351,11 @@
       <c r="P65" t="s">
         <v>32</v>
       </c>
-      <c r="Q65" t="s">
-        <v>36</v>
-      </c>
       <c r="T65" s="1">
-        <v>45701</v>
+        <v>45768</v>
       </c>
       <c r="W65" s="1">
-        <v>45717</v>
+        <v>45769</v>
       </c>
       <c r="X65" s="2">
         <v>0</v>
@@ -5389,13 +5366,13 @@
         <v>45808</v>
       </c>
       <c r="B66" t="s">
-        <v>181</v>
+        <v>105</v>
       </c>
       <c r="C66" t="s">
-        <v>182</v>
+        <v>106</v>
       </c>
       <c r="D66" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="E66" t="s">
         <v>59</v>
@@ -5403,11 +5380,17 @@
       <c r="F66" t="s">
         <v>41</v>
       </c>
-      <c r="H66">
-        <v>10000</v>
+      <c r="J66" t="s">
+        <v>28</v>
+      </c>
+      <c r="K66" t="s">
+        <v>29</v>
+      </c>
+      <c r="L66" t="s">
+        <v>30</v>
       </c>
       <c r="M66" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O66">
         <v>90113131698</v>
@@ -5415,11 +5398,17 @@
       <c r="P66" t="s">
         <v>32</v>
       </c>
+      <c r="Q66" t="s">
+        <v>107</v>
+      </c>
       <c r="T66" s="1">
-        <v>45768</v>
+        <v>45712</v>
+      </c>
+      <c r="U66" s="1">
+        <v>45712</v>
       </c>
       <c r="W66" s="1">
-        <v>45769</v>
+        <v>45717</v>
       </c>
       <c r="X66" s="2">
         <v>0</v>
@@ -5430,31 +5419,37 @@
         <v>45808</v>
       </c>
       <c r="B67" t="s">
-        <v>105</v>
+        <v>136</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
+        <v>137</v>
       </c>
       <c r="D67" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="E67" t="s">
         <v>59</v>
       </c>
       <c r="F67" t="s">
-        <v>41</v>
+        <v>45</v>
+      </c>
+      <c r="G67">
+        <v>0</v>
+      </c>
+      <c r="H67">
+        <v>0</v>
+      </c>
+      <c r="I67">
+        <v>8000</v>
       </c>
       <c r="J67" t="s">
         <v>28</v>
       </c>
-      <c r="K67" t="s">
-        <v>29</v>
-      </c>
       <c r="L67" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="M67" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O67">
         <v>90113131698</v>
@@ -5463,13 +5458,16 @@
         <v>32</v>
       </c>
       <c r="Q67" t="s">
-        <v>107</v>
+        <v>102</v>
+      </c>
+      <c r="S67" s="1">
+        <v>45869</v>
       </c>
       <c r="T67" s="1">
-        <v>45712</v>
+        <v>45716</v>
       </c>
       <c r="U67" s="1">
-        <v>45712</v>
+        <v>45691</v>
       </c>
       <c r="W67" s="1">
         <v>45717</v>
@@ -5483,37 +5481,34 @@
         <v>45808</v>
       </c>
       <c r="B68" t="s">
-        <v>136</v>
+        <v>99</v>
       </c>
       <c r="C68" t="s">
-        <v>137</v>
+        <v>100</v>
       </c>
       <c r="D68" t="s">
-        <v>73</v>
-      </c>
-      <c r="E68" t="s">
-        <v>59</v>
+        <v>101</v>
       </c>
       <c r="F68" t="s">
-        <v>45</v>
-      </c>
-      <c r="G68">
-        <v>0</v>
-      </c>
-      <c r="H68">
-        <v>0</v>
+        <v>27</v>
       </c>
       <c r="I68">
-        <v>8000</v>
+        <v>7500</v>
       </c>
       <c r="J68" t="s">
         <v>28</v>
       </c>
+      <c r="K68" t="s">
+        <v>29</v>
+      </c>
       <c r="L68" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="M68" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="N68" t="s">
+        <v>42</v>
       </c>
       <c r="O68">
         <v>90113131698</v>
@@ -5524,14 +5519,11 @@
       <c r="Q68" t="s">
         <v>102</v>
       </c>
-      <c r="S68" s="1">
-        <v>45869</v>
+      <c r="R68" s="1">
+        <v>45740</v>
       </c>
       <c r="T68" s="1">
-        <v>45716</v>
-      </c>
-      <c r="U68" s="1">
-        <v>45691</v>
+        <v>45712</v>
       </c>
       <c r="W68" s="1">
         <v>45717</v>
@@ -5545,34 +5537,37 @@
         <v>45808</v>
       </c>
       <c r="B69" t="s">
-        <v>99</v>
+        <v>255</v>
       </c>
       <c r="C69" t="s">
-        <v>100</v>
+        <v>256</v>
       </c>
       <c r="D69" t="s">
-        <v>101</v>
+        <v>200</v>
+      </c>
+      <c r="E69" t="s">
+        <v>59</v>
       </c>
       <c r="F69" t="s">
-        <v>27</v>
-      </c>
-      <c r="I69">
-        <v>7500</v>
+        <v>60</v>
+      </c>
+      <c r="G69">
+        <v>652.42999999999995</v>
       </c>
       <c r="J69" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="K69" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="L69" t="s">
         <v>30</v>
       </c>
       <c r="M69" t="s">
-        <v>266</v>
+        <v>69</v>
       </c>
       <c r="N69" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="O69">
         <v>90113131698</v>
@@ -5580,17 +5575,8 @@
       <c r="P69" t="s">
         <v>32</v>
       </c>
-      <c r="Q69" t="s">
-        <v>102</v>
-      </c>
-      <c r="R69" s="1">
-        <v>45740</v>
-      </c>
       <c r="T69" s="1">
-        <v>45712</v>
-      </c>
-      <c r="W69" s="1">
-        <v>45717</v>
+        <v>45832</v>
       </c>
       <c r="X69" s="2">
         <v>0</v>
@@ -5601,22 +5587,19 @@
         <v>45808</v>
       </c>
       <c r="B70" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="C70" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D70" t="s">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="E70" t="s">
-        <v>59</v>
+        <v>241</v>
       </c>
       <c r="F70" t="s">
-        <v>60</v>
-      </c>
-      <c r="G70">
-        <v>652.42999999999995</v>
+        <v>45</v>
       </c>
       <c r="J70" t="s">
         <v>74</v>
@@ -5630,9 +5613,6 @@
       <c r="M70" t="s">
         <v>69</v>
       </c>
-      <c r="N70" t="s">
-        <v>31</v>
-      </c>
       <c r="O70">
         <v>90113131698</v>
       </c>
@@ -5651,19 +5631,25 @@
         <v>45808</v>
       </c>
       <c r="B71" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="C71" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="D71" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="E71" t="s">
-        <v>242</v>
+        <v>59</v>
       </c>
       <c r="F71" t="s">
-        <v>45</v>
+        <v>81</v>
+      </c>
+      <c r="G71">
+        <v>619.94000000000005</v>
+      </c>
+      <c r="H71">
+        <v>350</v>
       </c>
       <c r="J71" t="s">
         <v>74</v>
@@ -5695,10 +5681,10 @@
         <v>45808</v>
       </c>
       <c r="B72" t="s">
-        <v>246</v>
+        <v>249</v>
       </c>
       <c r="C72" t="s">
-        <v>247</v>
+        <v>250</v>
       </c>
       <c r="D72" t="s">
         <v>200</v>
@@ -5707,13 +5693,7 @@
         <v>59</v>
       </c>
       <c r="F72" t="s">
-        <v>81</v>
-      </c>
-      <c r="G72">
-        <v>619.94000000000005</v>
-      </c>
-      <c r="H72">
-        <v>350</v>
+        <v>60</v>
       </c>
       <c r="J72" t="s">
         <v>74</v>
@@ -5727,6 +5707,9 @@
       <c r="M72" t="s">
         <v>69</v>
       </c>
+      <c r="N72" t="s">
+        <v>31</v>
+      </c>
       <c r="O72">
         <v>90113131698</v>
       </c>
@@ -5745,10 +5728,10 @@
         <v>45808</v>
       </c>
       <c r="B73" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="C73" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
       <c r="D73" t="s">
         <v>200</v>
@@ -5759,6 +5742,12 @@
       <c r="F73" t="s">
         <v>60</v>
       </c>
+      <c r="G73">
+        <v>1588.04</v>
+      </c>
+      <c r="H73">
+        <v>62164</v>
+      </c>
       <c r="J73" t="s">
         <v>74</v>
       </c>
@@ -5792,25 +5781,19 @@
         <v>45808</v>
       </c>
       <c r="B74" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="C74" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
       <c r="D74" t="s">
-        <v>200</v>
+        <v>240</v>
       </c>
       <c r="E74" t="s">
-        <v>59</v>
+        <v>241</v>
       </c>
       <c r="F74" t="s">
-        <v>60</v>
-      </c>
-      <c r="G74">
-        <v>1588.04</v>
-      </c>
-      <c r="H74">
-        <v>62164</v>
+        <v>41</v>
       </c>
       <c r="J74" t="s">
         <v>74</v>
@@ -5819,14 +5802,11 @@
         <v>68</v>
       </c>
       <c r="L74" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="M74" t="s">
         <v>69</v>
       </c>
-      <c r="N74" t="s">
-        <v>31</v>
-      </c>
       <c r="O74">
         <v>90113131698</v>
       </c>
@@ -5845,19 +5825,25 @@
         <v>45808</v>
       </c>
       <c r="B75" t="s">
-        <v>264</v>
+        <v>261</v>
       </c>
       <c r="C75" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="D75" t="s">
-        <v>241</v>
+        <v>200</v>
       </c>
       <c r="E75" t="s">
-        <v>242</v>
+        <v>59</v>
       </c>
       <c r="F75" t="s">
-        <v>41</v>
+        <v>81</v>
+      </c>
+      <c r="G75">
+        <v>119</v>
+      </c>
+      <c r="H75">
+        <v>714.11</v>
       </c>
       <c r="J75" t="s">
         <v>74</v>
@@ -5866,7 +5852,7 @@
         <v>68</v>
       </c>
       <c r="L75" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="M75" t="s">
         <v>69</v>
@@ -5889,10 +5875,10 @@
         <v>45808</v>
       </c>
       <c r="B76" t="s">
-        <v>262</v>
+        <v>247</v>
       </c>
       <c r="C76" t="s">
-        <v>263</v>
+        <v>248</v>
       </c>
       <c r="D76" t="s">
         <v>200</v>
@@ -5904,10 +5890,7 @@
         <v>81</v>
       </c>
       <c r="G76">
-        <v>119</v>
-      </c>
-      <c r="H76">
-        <v>714.11</v>
+        <v>2055.4899999999998</v>
       </c>
       <c r="J76" t="s">
         <v>74</v>
@@ -5921,6 +5904,9 @@
       <c r="M76" t="s">
         <v>69</v>
       </c>
+      <c r="N76" t="s">
+        <v>31</v>
+      </c>
       <c r="O76">
         <v>90113131698</v>
       </c>
@@ -5939,37 +5925,34 @@
         <v>45808</v>
       </c>
       <c r="B77" t="s">
-        <v>248</v>
+        <v>154</v>
       </c>
       <c r="C77" t="s">
-        <v>249</v>
+        <v>155</v>
       </c>
       <c r="D77" t="s">
-        <v>200</v>
+        <v>67</v>
       </c>
       <c r="E77" t="s">
         <v>59</v>
       </c>
       <c r="F77" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G77">
-        <v>2055.4899999999998</v>
+        <v>4000</v>
+      </c>
+      <c r="H77">
+        <v>14000</v>
+      </c>
+      <c r="I77">
+        <v>20000</v>
       </c>
       <c r="J77" t="s">
-        <v>74</v>
-      </c>
-      <c r="K77" t="s">
-        <v>68</v>
-      </c>
-      <c r="L77" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="M77" t="s">
-        <v>69</v>
-      </c>
-      <c r="N77" t="s">
-        <v>31</v>
+        <v>265</v>
       </c>
       <c r="O77">
         <v>90113131698</v>
@@ -5977,8 +5960,20 @@
       <c r="P77" t="s">
         <v>32</v>
       </c>
+      <c r="Q77" t="s">
+        <v>36</v>
+      </c>
+      <c r="S77" s="1">
+        <v>45869</v>
+      </c>
       <c r="T77" s="1">
-        <v>45832</v>
+        <v>45747</v>
+      </c>
+      <c r="U77" s="1">
+        <v>45810</v>
+      </c>
+      <c r="W77" s="1">
+        <v>45785</v>
       </c>
       <c r="X77" s="2">
         <v>0</v>
@@ -5989,34 +5984,28 @@
         <v>45808</v>
       </c>
       <c r="B78" t="s">
-        <v>154</v>
+        <v>167</v>
       </c>
       <c r="C78" t="s">
-        <v>155</v>
+        <v>270</v>
       </c>
       <c r="D78" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="E78" t="s">
         <v>59</v>
       </c>
       <c r="F78" t="s">
-        <v>60</v>
-      </c>
-      <c r="G78">
-        <v>4000</v>
-      </c>
-      <c r="H78">
-        <v>14000</v>
-      </c>
-      <c r="I78">
-        <v>20000</v>
+        <v>41</v>
       </c>
       <c r="J78" t="s">
         <v>28</v>
       </c>
+      <c r="K78" t="s">
+        <v>29</v>
+      </c>
       <c r="M78" t="s">
-        <v>266</v>
+        <v>69</v>
       </c>
       <c r="O78">
         <v>90113131698</v>
@@ -6024,20 +6013,11 @@
       <c r="P78" t="s">
         <v>32</v>
       </c>
-      <c r="Q78" t="s">
-        <v>36</v>
-      </c>
-      <c r="S78" s="1">
-        <v>45869</v>
-      </c>
       <c r="T78" s="1">
-        <v>45747</v>
-      </c>
-      <c r="U78" s="1">
-        <v>45810</v>
+        <v>45757</v>
       </c>
       <c r="W78" s="1">
-        <v>45785</v>
+        <v>45758</v>
       </c>
       <c r="X78" s="2">
         <v>0</v>
@@ -6048,13 +6028,13 @@
         <v>45808</v>
       </c>
       <c r="B79" t="s">
-        <v>167</v>
+        <v>91</v>
       </c>
       <c r="C79" t="s">
-        <v>271</v>
+        <v>92</v>
       </c>
       <c r="D79" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="E79" t="s">
         <v>59</v>
@@ -6062,14 +6042,23 @@
       <c r="F79" t="s">
         <v>41</v>
       </c>
+      <c r="G79">
+        <v>5000</v>
+      </c>
       <c r="J79" t="s">
         <v>28</v>
       </c>
       <c r="K79" t="s">
         <v>29</v>
       </c>
+      <c r="L79" t="s">
+        <v>30</v>
+      </c>
       <c r="M79" t="s">
-        <v>69</v>
+        <v>265</v>
+      </c>
+      <c r="N79" t="s">
+        <v>42</v>
       </c>
       <c r="O79">
         <v>90113131698</v>
@@ -6077,11 +6066,14 @@
       <c r="P79" t="s">
         <v>32</v>
       </c>
+      <c r="Q79" t="s">
+        <v>36</v>
+      </c>
       <c r="T79" s="1">
-        <v>45757</v>
+        <v>45701</v>
       </c>
       <c r="W79" s="1">
-        <v>45758</v>
+        <v>45749</v>
       </c>
       <c r="X79" s="2">
         <v>0</v>
@@ -6092,23 +6084,20 @@
         <v>45808</v>
       </c>
       <c r="B80" t="s">
-        <v>91</v>
+        <v>189</v>
       </c>
       <c r="C80" t="s">
-        <v>92</v>
+        <v>190</v>
       </c>
       <c r="D80" t="s">
-        <v>67</v>
+        <v>191</v>
       </c>
       <c r="E80" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="F80" t="s">
         <v>41</v>
       </c>
-      <c r="G80">
-        <v>5000</v>
-      </c>
       <c r="J80" t="s">
         <v>28</v>
       </c>
@@ -6119,7 +6108,7 @@
         <v>30</v>
       </c>
       <c r="M80" t="s">
-        <v>266</v>
+        <v>69</v>
       </c>
       <c r="N80" t="s">
         <v>42</v>
@@ -6130,14 +6119,11 @@
       <c r="P80" t="s">
         <v>32</v>
       </c>
-      <c r="Q80" t="s">
-        <v>36</v>
-      </c>
       <c r="T80" s="1">
-        <v>45701</v>
+        <v>45768</v>
       </c>
       <c r="W80" s="1">
-        <v>45749</v>
+        <v>45769</v>
       </c>
       <c r="X80" s="2">
         <v>0</v>
@@ -6148,19 +6134,25 @@
         <v>45808</v>
       </c>
       <c r="B81" t="s">
-        <v>189</v>
+        <v>133</v>
       </c>
       <c r="C81" t="s">
-        <v>190</v>
+        <v>134</v>
       </c>
       <c r="D81" t="s">
-        <v>191</v>
+        <v>25</v>
       </c>
       <c r="E81" t="s">
         <v>26</v>
       </c>
       <c r="F81" t="s">
-        <v>41</v>
+        <v>60</v>
+      </c>
+      <c r="G81">
+        <v>0</v>
+      </c>
+      <c r="H81">
+        <v>14000</v>
       </c>
       <c r="J81" t="s">
         <v>28</v>
@@ -6169,13 +6161,13 @@
         <v>29</v>
       </c>
       <c r="L81" t="s">
-        <v>30</v>
+        <v>75</v>
       </c>
       <c r="M81" t="s">
-        <v>69</v>
+        <v>265</v>
       </c>
       <c r="N81" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="O81">
         <v>90113131698</v>
@@ -6183,11 +6175,17 @@
       <c r="P81" t="s">
         <v>32</v>
       </c>
+      <c r="Q81" t="s">
+        <v>135</v>
+      </c>
+      <c r="S81" s="1">
+        <v>45791</v>
+      </c>
       <c r="T81" s="1">
-        <v>45768</v>
+        <v>45715</v>
       </c>
       <c r="W81" s="1">
-        <v>45769</v>
+        <v>45749</v>
       </c>
       <c r="X81" s="2">
         <v>0</v>
@@ -6198,10 +6196,10 @@
         <v>45808</v>
       </c>
       <c r="B82" t="s">
-        <v>133</v>
+        <v>234</v>
       </c>
       <c r="C82" t="s">
-        <v>134</v>
+        <v>235</v>
       </c>
       <c r="D82" t="s">
         <v>25</v>
@@ -6210,13 +6208,10 @@
         <v>26</v>
       </c>
       <c r="F82" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="G82">
-        <v>0</v>
-      </c>
-      <c r="H82">
-        <v>14000</v>
+        <v>1777</v>
       </c>
       <c r="J82" t="s">
         <v>28</v>
@@ -6228,10 +6223,7 @@
         <v>75</v>
       </c>
       <c r="M82" t="s">
-        <v>266</v>
-      </c>
-      <c r="N82" t="s">
-        <v>31</v>
+        <v>265</v>
       </c>
       <c r="O82">
         <v>90113131698</v>
@@ -6242,14 +6234,17 @@
       <c r="Q82" t="s">
         <v>135</v>
       </c>
+      <c r="R82" s="1">
+        <v>45807</v>
+      </c>
       <c r="S82" s="1">
-        <v>45791</v>
+        <v>45814</v>
       </c>
       <c r="T82" s="1">
-        <v>45715</v>
+        <v>45814</v>
       </c>
       <c r="W82" s="1">
-        <v>45749</v>
+        <v>45815</v>
       </c>
       <c r="X82" s="2">
         <v>0</v>
@@ -6260,10 +6255,10 @@
         <v>45808</v>
       </c>
       <c r="B83" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="C83" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="D83" t="s">
         <v>25</v>
@@ -6272,10 +6267,10 @@
         <v>26</v>
       </c>
       <c r="F83" t="s">
-        <v>27</v>
-      </c>
-      <c r="G83">
-        <v>1777</v>
+        <v>81</v>
+      </c>
+      <c r="H83">
+        <v>3000</v>
       </c>
       <c r="J83" t="s">
         <v>28</v>
@@ -6284,10 +6279,13 @@
         <v>29</v>
       </c>
       <c r="L83" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
       <c r="M83" t="s">
-        <v>266</v>
+        <v>265</v>
+      </c>
+      <c r="N83" t="s">
+        <v>31</v>
       </c>
       <c r="O83">
         <v>90113131698</v>
@@ -6298,12 +6296,6 @@
       <c r="Q83" t="s">
         <v>135</v>
       </c>
-      <c r="R83" s="1">
-        <v>45807</v>
-      </c>
-      <c r="S83" s="1">
-        <v>45814</v>
-      </c>
       <c r="T83" s="1">
         <v>45814</v>
       </c>
@@ -6319,37 +6311,19 @@
         <v>45808</v>
       </c>
       <c r="B84" t="s">
-        <v>237</v>
+        <v>198</v>
       </c>
       <c r="C84" t="s">
-        <v>238</v>
+        <v>199</v>
       </c>
       <c r="D84" t="s">
-        <v>25</v>
+        <v>200</v>
       </c>
       <c r="E84" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F84" t="s">
-        <v>81</v>
-      </c>
-      <c r="H84">
-        <v>3000</v>
-      </c>
-      <c r="J84" t="s">
-        <v>28</v>
-      </c>
-      <c r="K84" t="s">
-        <v>29</v>
-      </c>
-      <c r="L84" t="s">
-        <v>30</v>
-      </c>
-      <c r="M84" t="s">
-        <v>266</v>
-      </c>
-      <c r="N84" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
       <c r="O84">
         <v>90113131698</v>
@@ -6357,17 +6331,14 @@
       <c r="P84" t="s">
         <v>32</v>
       </c>
-      <c r="Q84" t="s">
-        <v>135</v>
-      </c>
       <c r="T84" s="1">
-        <v>45814</v>
+        <v>45790</v>
       </c>
       <c r="W84" s="1">
-        <v>45815</v>
+        <v>45791</v>
       </c>
       <c r="X84" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="85" spans="1:24" x14ac:dyDescent="0.25">
@@ -6375,19 +6346,43 @@
         <v>45808</v>
       </c>
       <c r="B85" t="s">
-        <v>198</v>
+        <v>125</v>
       </c>
       <c r="C85" t="s">
-        <v>199</v>
+        <v>126</v>
       </c>
       <c r="D85" t="s">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="E85" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="F85" t="s">
-        <v>41</v>
+        <v>81</v>
+      </c>
+      <c r="G85">
+        <v>5328</v>
+      </c>
+      <c r="H85">
+        <v>28400</v>
+      </c>
+      <c r="I85">
+        <v>3000</v>
+      </c>
+      <c r="J85" t="s">
+        <v>28</v>
+      </c>
+      <c r="K85" t="s">
+        <v>29</v>
+      </c>
+      <c r="L85" t="s">
+        <v>30</v>
+      </c>
+      <c r="M85" t="s">
+        <v>265</v>
+      </c>
+      <c r="N85" t="s">
+        <v>42</v>
       </c>
       <c r="O85">
         <v>90113131698</v>
@@ -6395,11 +6390,17 @@
       <c r="P85" t="s">
         <v>32</v>
       </c>
+      <c r="Q85" t="s">
+        <v>127</v>
+      </c>
+      <c r="S85" s="1">
+        <v>45812</v>
+      </c>
       <c r="T85" s="1">
-        <v>45790</v>
+        <v>45715</v>
       </c>
       <c r="W85" s="1">
-        <v>45791</v>
+        <v>45717</v>
       </c>
       <c r="X85" s="2">
         <v>0</v>
@@ -6410,10 +6411,10 @@
         <v>45808</v>
       </c>
       <c r="B86" t="s">
-        <v>125</v>
+        <v>158</v>
       </c>
       <c r="C86" t="s">
-        <v>126</v>
+        <v>159</v>
       </c>
       <c r="D86" t="s">
         <v>25</v>
@@ -6425,10 +6426,10 @@
         <v>81</v>
       </c>
       <c r="G86">
-        <v>5328</v>
+        <v>1800</v>
       </c>
       <c r="H86">
-        <v>28400</v>
+        <v>2500</v>
       </c>
       <c r="I86">
         <v>3000</v>
@@ -6443,7 +6444,7 @@
         <v>30</v>
       </c>
       <c r="M86" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N86" t="s">
         <v>42</v>
@@ -6455,16 +6456,16 @@
         <v>32</v>
       </c>
       <c r="Q86" t="s">
-        <v>127</v>
+        <v>160</v>
       </c>
       <c r="S86" s="1">
-        <v>45812</v>
+        <v>45786</v>
       </c>
       <c r="T86" s="1">
-        <v>45715</v>
+        <v>45747</v>
       </c>
       <c r="W86" s="1">
-        <v>45717</v>
+        <v>45749</v>
       </c>
       <c r="X86" s="2">
         <v>0</v>
@@ -6475,10 +6476,10 @@
         <v>45808</v>
       </c>
       <c r="B87" t="s">
-        <v>158</v>
+        <v>145</v>
       </c>
       <c r="C87" t="s">
-        <v>159</v>
+        <v>146</v>
       </c>
       <c r="D87" t="s">
         <v>25</v>
@@ -6487,16 +6488,13 @@
         <v>26</v>
       </c>
       <c r="F87" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G87">
-        <v>1800</v>
+        <v>0</v>
       </c>
       <c r="H87">
-        <v>2500</v>
-      </c>
-      <c r="I87">
-        <v>3000</v>
+        <v>0</v>
       </c>
       <c r="J87" t="s">
         <v>28</v>
@@ -6505,10 +6503,10 @@
         <v>29</v>
       </c>
       <c r="L87" t="s">
-        <v>30</v>
+        <v>147</v>
       </c>
       <c r="M87" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N87" t="s">
         <v>42</v>
@@ -6519,17 +6517,17 @@
       <c r="P87" t="s">
         <v>32</v>
       </c>
-      <c r="Q87" t="s">
-        <v>160</v>
-      </c>
       <c r="S87" s="1">
-        <v>45786</v>
+        <v>45785</v>
       </c>
       <c r="T87" s="1">
-        <v>45747</v>
+        <v>45716</v>
+      </c>
+      <c r="U87" s="1">
+        <v>45826</v>
       </c>
       <c r="W87" s="1">
-        <v>45749</v>
+        <v>45790</v>
       </c>
       <c r="X87" s="2">
         <v>0</v>
@@ -6540,10 +6538,10 @@
         <v>45808</v>
       </c>
       <c r="B88" t="s">
-        <v>145</v>
+        <v>123</v>
       </c>
       <c r="C88" t="s">
-        <v>146</v>
+        <v>124</v>
       </c>
       <c r="D88" t="s">
         <v>25</v>
@@ -6555,10 +6553,13 @@
         <v>60</v>
       </c>
       <c r="G88">
-        <v>0</v>
+        <v>8000</v>
       </c>
       <c r="H88">
-        <v>0</v>
+        <v>5000</v>
+      </c>
+      <c r="I88">
+        <v>5000</v>
       </c>
       <c r="J88" t="s">
         <v>28</v>
@@ -6567,13 +6568,13 @@
         <v>29</v>
       </c>
       <c r="L88" t="s">
-        <v>147</v>
+        <v>30</v>
       </c>
       <c r="M88" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N88" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="O88">
         <v>90113131698</v>
@@ -6581,17 +6582,20 @@
       <c r="P88" t="s">
         <v>32</v>
       </c>
+      <c r="Q88" t="s">
+        <v>36</v>
+      </c>
       <c r="S88" s="1">
-        <v>45785</v>
+        <v>45782</v>
       </c>
       <c r="T88" s="1">
-        <v>45716</v>
+        <v>45715</v>
       </c>
       <c r="U88" s="1">
-        <v>45826</v>
+        <v>45772</v>
       </c>
       <c r="W88" s="1">
-        <v>45790</v>
+        <v>45749</v>
       </c>
       <c r="X88" s="2">
         <v>0</v>
@@ -6602,10 +6606,10 @@
         <v>45808</v>
       </c>
       <c r="B89" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="C89" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="D89" t="s">
         <v>25</v>
@@ -6617,13 +6621,10 @@
         <v>60</v>
       </c>
       <c r="G89">
-        <v>8000</v>
+        <v>18467</v>
       </c>
       <c r="H89">
-        <v>5000</v>
-      </c>
-      <c r="I89">
-        <v>5000</v>
+        <v>40000</v>
       </c>
       <c r="J89" t="s">
         <v>28</v>
@@ -6635,7 +6636,7 @@
         <v>30</v>
       </c>
       <c r="M89" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="N89" t="s">
         <v>31</v>
@@ -6650,19 +6651,19 @@
         <v>36</v>
       </c>
       <c r="S89" s="1">
-        <v>45782</v>
+        <v>45792</v>
       </c>
       <c r="T89" s="1">
-        <v>45715</v>
+        <v>45716</v>
       </c>
       <c r="U89" s="1">
+        <v>45722</v>
+      </c>
+      <c r="W89" s="1">
         <v>45772</v>
       </c>
-      <c r="W89" s="1">
-        <v>45749</v>
-      </c>
       <c r="X89" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="90" spans="1:24" x14ac:dyDescent="0.25">
@@ -6670,40 +6671,31 @@
         <v>45808</v>
       </c>
       <c r="B90" t="s">
-        <v>138</v>
+        <v>82</v>
       </c>
       <c r="C90" t="s">
-        <v>139</v>
+        <v>83</v>
       </c>
       <c r="D90" t="s">
-        <v>25</v>
+        <v>73</v>
       </c>
       <c r="E90" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F90" t="s">
-        <v>60</v>
-      </c>
-      <c r="G90">
-        <v>18467</v>
-      </c>
-      <c r="H90">
-        <v>40000</v>
+        <v>41</v>
       </c>
       <c r="J90" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="K90" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="L90" t="s">
         <v>30</v>
       </c>
       <c r="M90" t="s">
-        <v>266</v>
-      </c>
-      <c r="N90" t="s">
-        <v>31</v>
+        <v>265</v>
       </c>
       <c r="O90">
         <v>90113131698</v>
@@ -6711,20 +6703,11 @@
       <c r="P90" t="s">
         <v>32</v>
       </c>
-      <c r="Q90" t="s">
-        <v>36</v>
-      </c>
-      <c r="S90" s="1">
-        <v>45792</v>
-      </c>
       <c r="T90" s="1">
-        <v>45716</v>
-      </c>
-      <c r="U90" s="1">
-        <v>45722</v>
+        <v>45694</v>
       </c>
       <c r="W90" s="1">
-        <v>45772</v>
+        <v>45717</v>
       </c>
       <c r="X90" s="2">
         <v>0</v>
@@ -6735,22 +6718,25 @@
         <v>45808</v>
       </c>
       <c r="B91" t="s">
-        <v>82</v>
+        <v>110</v>
       </c>
       <c r="C91" t="s">
-        <v>83</v>
+        <v>111</v>
       </c>
       <c r="D91" t="s">
-        <v>73</v>
+        <v>25</v>
       </c>
       <c r="E91" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="F91" t="s">
-        <v>41</v>
+        <v>35</v>
+      </c>
+      <c r="H91">
+        <v>21802</v>
       </c>
       <c r="J91" t="s">
-        <v>74</v>
+        <v>28</v>
       </c>
       <c r="K91" t="s">
         <v>68</v>
@@ -6759,7 +6745,10 @@
         <v>30</v>
       </c>
       <c r="M91" t="s">
-        <v>266</v>
+        <v>69</v>
+      </c>
+      <c r="N91" t="s">
+        <v>42</v>
       </c>
       <c r="O91">
         <v>90113131698</v>
@@ -6767,11 +6756,20 @@
       <c r="P91" t="s">
         <v>32</v>
       </c>
+      <c r="Q91" t="s">
+        <v>36</v>
+      </c>
+      <c r="S91" s="1">
+        <v>45777</v>
+      </c>
       <c r="T91" s="1">
-        <v>45694</v>
+        <v>45715</v>
+      </c>
+      <c r="U91" s="1">
+        <v>45712</v>
       </c>
       <c r="W91" s="1">
-        <v>45717</v>
+        <v>45749</v>
       </c>
       <c r="X91" s="2">
         <v>0</v>
@@ -6782,10 +6780,10 @@
         <v>45808</v>
       </c>
       <c r="B92" t="s">
-        <v>110</v>
+        <v>161</v>
       </c>
       <c r="C92" t="s">
-        <v>111</v>
+        <v>271</v>
       </c>
       <c r="D92" t="s">
         <v>25</v>
@@ -6794,25 +6792,31 @@
         <v>26</v>
       </c>
       <c r="F92" t="s">
-        <v>35</v>
+        <v>81</v>
+      </c>
+      <c r="G92">
+        <v>8000</v>
       </c>
       <c r="H92">
-        <v>21802</v>
+        <v>10000</v>
+      </c>
+      <c r="I92">
+        <v>5000</v>
       </c>
       <c r="J92" t="s">
         <v>28</v>
       </c>
       <c r="K92" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="L92" t="s">
         <v>30</v>
       </c>
       <c r="M92" t="s">
-        <v>69</v>
+        <v>265</v>
       </c>
       <c r="N92" t="s">
-        <v>42</v>
+        <v>31</v>
       </c>
       <c r="O92">
         <v>90113131698</v>
@@ -6824,16 +6828,19 @@
         <v>36</v>
       </c>
       <c r="S92" s="1">
-        <v>45777</v>
+        <v>45806</v>
       </c>
       <c r="T92" s="1">
-        <v>45715</v>
+        <v>45756</v>
       </c>
       <c r="U92" s="1">
-        <v>45712</v>
+        <v>45807</v>
+      </c>
+      <c r="V92" s="1">
+        <v>45789</v>
       </c>
       <c r="W92" s="1">
-        <v>45749</v>
+        <v>45757</v>
       </c>
       <c r="X92" s="2">
         <v>0</v>
@@ -6844,43 +6851,37 @@
         <v>45808</v>
       </c>
       <c r="B93" t="s">
-        <v>161</v>
+        <v>168</v>
       </c>
       <c r="C93" t="s">
-        <v>272</v>
+        <v>169</v>
       </c>
       <c r="D93" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E93" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F93" t="s">
-        <v>81</v>
+        <v>60</v>
       </c>
       <c r="G93">
-        <v>8000</v>
+        <v>2604</v>
       </c>
       <c r="H93">
-        <v>10000</v>
-      </c>
-      <c r="I93">
-        <v>5000</v>
+        <v>13522</v>
       </c>
       <c r="J93" t="s">
         <v>28</v>
       </c>
       <c r="K93" t="s">
-        <v>29</v>
+        <v>68</v>
       </c>
       <c r="L93" t="s">
         <v>30</v>
       </c>
       <c r="M93" t="s">
-        <v>266</v>
-      </c>
-      <c r="N93" t="s">
-        <v>31</v>
+        <v>69</v>
       </c>
       <c r="O93">
         <v>90113131698</v>
@@ -6889,22 +6890,16 @@
         <v>32</v>
       </c>
       <c r="Q93" t="s">
-        <v>36</v>
+        <v>170</v>
       </c>
       <c r="S93" s="1">
-        <v>45806</v>
+        <v>45869</v>
       </c>
       <c r="T93" s="1">
-        <v>45756</v>
-      </c>
-      <c r="U93" s="1">
-        <v>45807</v>
-      </c>
-      <c r="V93" s="1">
-        <v>45789</v>
+        <v>45757</v>
       </c>
       <c r="W93" s="1">
-        <v>45757</v>
+        <v>45815</v>
       </c>
       <c r="X93" s="2">
         <v>0</v>
@@ -6915,37 +6910,31 @@
         <v>45808</v>
       </c>
       <c r="B94" t="s">
-        <v>168</v>
+        <v>37</v>
       </c>
       <c r="C94" t="s">
-        <v>169</v>
+        <v>38</v>
       </c>
       <c r="D94" t="s">
-        <v>67</v>
+        <v>25</v>
       </c>
       <c r="E94" t="s">
-        <v>59</v>
+        <v>26</v>
       </c>
       <c r="F94" t="s">
-        <v>60</v>
-      </c>
-      <c r="G94">
-        <v>2604</v>
-      </c>
-      <c r="H94">
-        <v>13522</v>
+        <v>35</v>
       </c>
       <c r="J94" t="s">
         <v>28</v>
       </c>
       <c r="K94" t="s">
-        <v>68</v>
+        <v>29</v>
       </c>
       <c r="L94" t="s">
         <v>30</v>
       </c>
       <c r="M94" t="s">
-        <v>69</v>
+        <v>265</v>
       </c>
       <c r="O94">
         <v>90113131698</v>
@@ -6954,16 +6943,13 @@
         <v>32</v>
       </c>
       <c r="Q94" t="s">
-        <v>170</v>
-      </c>
-      <c r="S94" s="1">
-        <v>45869</v>
+        <v>38</v>
       </c>
       <c r="T94" s="1">
-        <v>45757</v>
+        <v>45664</v>
       </c>
       <c r="W94" s="1">
-        <v>45815</v>
+        <v>45717</v>
       </c>
       <c r="X94" s="2">
         <v>0</v>
@@ -6974,19 +6960,25 @@
         <v>45808</v>
       </c>
       <c r="B95" t="s">
-        <v>37</v>
+        <v>221</v>
       </c>
       <c r="C95" t="s">
-        <v>38</v>
+        <v>222</v>
       </c>
       <c r="D95" t="s">
-        <v>25</v>
+        <v>67</v>
       </c>
       <c r="E95" t="s">
-        <v>26</v>
+        <v>59</v>
       </c>
       <c r="F95" t="s">
-        <v>35</v>
+        <v>60</v>
+      </c>
+      <c r="G95">
+        <v>11568</v>
+      </c>
+      <c r="H95">
+        <v>53295</v>
       </c>
       <c r="J95" t="s">
         <v>28</v>
@@ -6998,7 +6990,7 @@
         <v>30</v>
       </c>
       <c r="M95" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="O95">
         <v>90113131698</v>
@@ -7007,84 +6999,28 @@
         <v>32</v>
       </c>
       <c r="Q95" t="s">
-        <v>38</v>
+        <v>62</v>
+      </c>
+      <c r="S95" s="1">
+        <v>45838</v>
       </c>
       <c r="T95" s="1">
-        <v>45664</v>
+        <v>45814</v>
+      </c>
+      <c r="U95" s="1">
+        <v>45838</v>
       </c>
       <c r="W95" s="1">
-        <v>45717</v>
+        <v>45815</v>
       </c>
       <c r="X95" s="2">
         <v>0</v>
       </c>
     </row>
-    <row r="96" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A96" s="1">
-        <v>45808</v>
-      </c>
-      <c r="B96" t="s">
-        <v>222</v>
-      </c>
-      <c r="C96" t="s">
-        <v>223</v>
-      </c>
-      <c r="D96" t="s">
-        <v>67</v>
-      </c>
-      <c r="E96" t="s">
-        <v>59</v>
-      </c>
-      <c r="F96" t="s">
-        <v>60</v>
-      </c>
-      <c r="G96">
-        <v>11568</v>
-      </c>
-      <c r="H96">
-        <v>53295</v>
-      </c>
-      <c r="J96" t="s">
-        <v>28</v>
-      </c>
-      <c r="K96" t="s">
-        <v>29</v>
-      </c>
-      <c r="L96" t="s">
-        <v>30</v>
-      </c>
-      <c r="M96" t="s">
-        <v>266</v>
-      </c>
-      <c r="O96">
-        <v>90113131698</v>
-      </c>
-      <c r="P96" t="s">
-        <v>32</v>
-      </c>
-      <c r="Q96" t="s">
-        <v>62</v>
-      </c>
-      <c r="S96" s="1">
-        <v>45838</v>
-      </c>
-      <c r="T96" s="1">
-        <v>45814</v>
-      </c>
-      <c r="U96" s="1">
-        <v>45838</v>
-      </c>
-      <c r="W96" s="1">
-        <v>45815</v>
-      </c>
-      <c r="X96" s="2">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:X96" xr:uid="{00000000-0009-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X96">
-      <sortCondition ref="C1:C96"/>
+  <autoFilter ref="A1:X95" xr:uid="{00000000-0009-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:X95">
+      <sortCondition ref="C1:C95"/>
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>